<commit_message>
June data update (except national capacity data which is due Jul 21)
</commit_message>
<xml_diff>
--- a/data/New power capacity by province and type.xlsx
+++ b/data/New power capacity by province and type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\Rpackages\china_co2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEAB289-D2C2-4199-9F12-D9F129C0AF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C309091B-8C7F-49E7-A0D5-9267AD8171F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1577" yWindow="-103" windowWidth="31440" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4880" yWindow="1520" windowWidth="27540" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="China_ New Power Construction C" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="375">
   <si>
     <t>Name</t>
   </si>
@@ -1034,13 +1034,7 @@
     <t>Time Period</t>
   </si>
   <si>
-    <t>2008-12:2023-04</t>
-  </si>
-  <si>
     <t>2016-02:2022-12</t>
-  </si>
-  <si>
-    <t>2009-04:2023-04</t>
   </si>
   <si>
     <t>2009-10:2017-12</t>
@@ -1049,28 +1043,16 @@
     <t>2009-10:2022-12</t>
   </si>
   <si>
-    <t>2009-11:2023-04</t>
-  </si>
-  <si>
     <t>2016-02:2017-12</t>
   </si>
   <si>
     <t>2008-12:2022-12</t>
   </si>
   <si>
-    <t>2009-10:2023-04</t>
-  </si>
-  <si>
     <t>2010-11:2022-12</t>
   </si>
   <si>
-    <t>2010-10:2023-04</t>
-  </si>
-  <si>
     <t>2009-11:2022-12</t>
-  </si>
-  <si>
-    <t>2009-06:2023-04</t>
   </si>
   <si>
     <t>2009-04:2022-12</t>
@@ -1079,28 +1061,13 @@
     <t>2016-02:2020-12</t>
   </si>
   <si>
-    <t>2011-07:2022-12</t>
-  </si>
-  <si>
     <t>2008-12:2021-12</t>
-  </si>
-  <si>
-    <t>2009-05:2023-04</t>
   </si>
   <si>
     <t>2009-04:2017-12</t>
   </si>
   <si>
-    <t>2011-06:2023-04</t>
-  </si>
-  <si>
-    <t>2010-09:2023-04</t>
-  </si>
-  <si>
     <t>2015-06:2021-12</t>
-  </si>
-  <si>
-    <t>2010-11:2023-04</t>
   </si>
   <si>
     <t>2011-04:2022-12</t>
@@ -1115,45 +1082,6 @@
     <t>2009-10:2019-12</t>
   </si>
   <si>
-    <t>2015-03:2023-04</t>
-  </si>
-  <si>
-    <t>2014-02:2023-04</t>
-  </si>
-  <si>
-    <t>2014-04:2023-04</t>
-  </si>
-  <si>
-    <t>2013-05:2023-04</t>
-  </si>
-  <si>
-    <t>2013-04:2023-04</t>
-  </si>
-  <si>
-    <t>2013-10:2023-04</t>
-  </si>
-  <si>
-    <t>2013-07:2023-04</t>
-  </si>
-  <si>
-    <t>2014-06:2023-04</t>
-  </si>
-  <si>
-    <t>2014-08:2023-04</t>
-  </si>
-  <si>
-    <t>2015-02:2023-04</t>
-  </si>
-  <si>
-    <t>2015-07:2023-04</t>
-  </si>
-  <si>
-    <t>2015-12:2023-04</t>
-  </si>
-  <si>
-    <t>2015-05:2023-04</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -1163,13 +1091,7 @@
     <t>Update</t>
   </si>
   <si>
-    <t>2023-05-24</t>
-  </si>
-  <si>
     <t>2023-02-17</t>
-  </si>
-  <si>
-    <t>2023-05-25</t>
   </si>
   <si>
     <t>2018-01-19</t>
@@ -1185,6 +1107,81 @@
   </si>
   <si>
     <t>2020-02-24</t>
+  </si>
+  <si>
+    <t>2008-12:2023-05</t>
+  </si>
+  <si>
+    <t>2009-04:2023-05</t>
+  </si>
+  <si>
+    <t>2009-11:2023-05</t>
+  </si>
+  <si>
+    <t>2009-10:2023-05</t>
+  </si>
+  <si>
+    <t>2010-10:2023-05</t>
+  </si>
+  <si>
+    <t>2009-06:2023-05</t>
+  </si>
+  <si>
+    <t>2011-07:2023-05</t>
+  </si>
+  <si>
+    <t>2009-05:2023-05</t>
+  </si>
+  <si>
+    <t>2011-06:2023-05</t>
+  </si>
+  <si>
+    <t>2010-09:2023-05</t>
+  </si>
+  <si>
+    <t>2010-11:2023-05</t>
+  </si>
+  <si>
+    <t>2015-03:2023-05</t>
+  </si>
+  <si>
+    <t>2014-02:2023-05</t>
+  </si>
+  <si>
+    <t>2014-04:2023-05</t>
+  </si>
+  <si>
+    <t>2013-05:2023-05</t>
+  </si>
+  <si>
+    <t>2013-04:2023-05</t>
+  </si>
+  <si>
+    <t>2013-10:2023-05</t>
+  </si>
+  <si>
+    <t>2013-07:2023-05</t>
+  </si>
+  <si>
+    <t>2014-06:2023-05</t>
+  </si>
+  <si>
+    <t>2014-08:2023-05</t>
+  </si>
+  <si>
+    <t>2015-02:2023-05</t>
+  </si>
+  <si>
+    <t>2015-07:2023-05</t>
+  </si>
+  <si>
+    <t>2015-12:2023-05</t>
+  </si>
+  <si>
+    <t>2015-05:2023-05</t>
+  </si>
+  <si>
+    <t>2023-06-29</t>
   </si>
 </sst>
 </file>
@@ -1585,10 +1582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FD159"/>
+  <dimension ref="A1:FD160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3532,1445 +3529,1445 @@
         <v>324</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="H6" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AP6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AS6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AT6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AU6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AW6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AX6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AY6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AZ6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BA6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BB6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BC6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BD6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BE6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="BF6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="BG6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="BH6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="BI6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BJ6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BK6" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="BL6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BM6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BN6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BO6" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="BP6" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="BQ6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BR6" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="BS6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BT6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BU6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BV6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BW6" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="BX6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BY6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="BZ6" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="CA6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="CB6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="CC6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="CD6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="CE6" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="CF6" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="CG6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="CH6" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="CI6" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="CJ6" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="CK6" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="CL6" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="CM6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="CN6" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="CO6" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="CP6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="CQ6" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="CR6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="CS6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="CT6" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="CU6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="CV6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="CW6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="CX6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="CY6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="CZ6" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="DA6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="DB6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="DC6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="DD6" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="DE6" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="DF6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="DG6" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="DH6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="DI6" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="DJ6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="DK6" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="DL6" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="DM6" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="DN6" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="DO6" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="DP6" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="V6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AE6" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="AF6" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AH6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AI6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="AJ6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AK6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AN6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AO6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AP6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AQ6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AR6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AS6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AT6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AU6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AV6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AW6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AX6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AY6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AZ6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BA6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BB6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BC6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BD6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="BE6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="BF6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="BG6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="BH6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="BI6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BJ6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BK6" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="BL6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="BM6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BN6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BO6" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="BP6" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="BQ6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BR6" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="BS6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BT6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BU6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BV6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BW6" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="BX6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BY6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="BZ6" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="CA6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="CB6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="CC6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="CD6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="CE6" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="CF6" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="CG6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="CH6" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="CI6" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="CJ6" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="CK6" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="CL6" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="CM6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="CN6" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="CO6" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="CP6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="CQ6" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="CR6" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="CS6" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="CT6" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="CU6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="CV6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="CW6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="CX6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="CY6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="CZ6" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="DA6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DB6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DC6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DD6" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="DE6" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="DF6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DG6" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="DH6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DI6" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="DJ6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DK6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DL6" s="4" t="s">
+      <c r="DQ6" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="DM6" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="DN6" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="DO6" s="4" t="s">
+      <c r="DR6" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="DP6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DQ6" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="DR6" s="4" t="s">
-        <v>331</v>
-      </c>
       <c r="DS6" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DT6" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DU6" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DV6" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DW6" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DX6" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DY6" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DZ6" s="4" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="EA6" s="4" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="EB6" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="EC6" s="4" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="ED6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="EE6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="EF6" s="4" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="EG6" s="4" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="EH6" s="4" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="EI6" s="4" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="EJ6" s="4" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="EK6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="EL6" s="4" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="EM6" s="4" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="EN6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="EO6" s="4" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="EP6" s="4" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="EQ6" s="4" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="ER6" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="ES6" s="4" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="ET6" s="4" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="EU6" s="4" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="EV6" s="4" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="EW6" s="4" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="EX6" s="4" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="EY6" s="4" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="EZ6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="FA6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="FB6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="FC6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="FD6" s="4" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:160" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AD7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AE7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AF7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AG7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AH7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AI7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AL7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AM7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AN7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AO7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AP7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AQ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AR7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AS7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AU7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AV7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AW7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AX7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AY7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AZ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BA7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BB7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BC7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BD7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BE7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BF7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BG7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BH7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BI7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BJ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BK7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BL7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BM7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BN7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BO7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BP7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BQ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BR7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BS7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BT7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BU7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BV7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BW7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BX7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BY7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="BZ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CA7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CB7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CC7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CD7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CE7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CF7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CG7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CH7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CI7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CJ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CK7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CL7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CM7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CN7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CO7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CP7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CQ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CR7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CS7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CT7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CU7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CV7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CW7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CX7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CY7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="CZ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DA7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DB7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DC7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DD7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DE7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DF7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DG7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DH7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DI7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DJ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DK7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DL7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DM7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DN7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DO7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DP7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DQ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DR7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DS7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DT7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DU7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DV7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DW7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DX7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DY7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="DZ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EA7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EB7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EC7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="ED7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EE7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EF7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EG7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EH7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EI7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EJ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EK7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EL7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EM7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EN7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EO7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EP7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EQ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="ER7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="ES7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="ET7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EU7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EV7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EW7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EX7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EY7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="EZ7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="FA7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="FB7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="FC7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="FD7" s="4" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:160" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="AF8" s="5" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="AG8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AH8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AM8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AN8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AO8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AP8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AQ8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AR8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AS8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AT8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AV8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AW8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AX8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AY8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AZ8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BA8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BB8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BC8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BD8" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="BE8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="BF8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="BG8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="BH8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="BI8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BJ8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BK8" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="BL8" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="BM8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BN8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BO8" s="5" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="BP8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BQ8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BR8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BS8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BT8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BU8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BV8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BW8" s="5" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="BX8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="BY8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="BZ8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="CA8" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="CB8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="CC8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CD8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CE8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CF8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CG8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="CH8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CI8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="CJ8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="CK8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CL8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CM8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CN8" s="5" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="CO8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="CP8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="CQ8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="CR8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="CS8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="CT8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="CU8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="CV8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="CW8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="CX8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="CY8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="CZ8" s="5" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="DA8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DB8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DC8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DD8" s="5" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="DE8" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="DF8" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DG8" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="DH8" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DI8" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="DJ8" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DK8" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DL8" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="DM8" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="DN8" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="DF8" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="DG8" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="DH8" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="DI8" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="DJ8" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="DK8" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="DL8" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="DM8" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="DN8" s="5" t="s">
-        <v>370</v>
-      </c>
       <c r="DO8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DP8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DQ8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DR8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DS8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DT8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DU8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DV8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DW8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DX8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DY8" s="5" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="DZ8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EA8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EB8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EC8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="ED8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EE8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EF8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EG8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EH8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EI8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EJ8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EK8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EL8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EM8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EN8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EO8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EP8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EQ8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="ER8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="ES8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="ET8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EU8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EV8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EW8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="EX8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="EY8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="EZ8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="FA8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="FB8" s="5" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="FC8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="FD8" s="5" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:160" x14ac:dyDescent="0.35">
@@ -77753,6 +77750,488 @@
       </c>
       <c r="FD159" s="3">
         <v>213</v>
+      </c>
+    </row>
+    <row r="160" spans="1:160" x14ac:dyDescent="0.35">
+      <c r="A160" s="2">
+        <v>45077</v>
+      </c>
+      <c r="B160" s="3">
+        <v>434</v>
+      </c>
+      <c r="C160" s="3">
+        <v>0</v>
+      </c>
+      <c r="D160" s="3">
+        <v>0</v>
+      </c>
+      <c r="E160" s="3">
+        <v>90</v>
+      </c>
+      <c r="F160" s="3">
+        <v>1</v>
+      </c>
+      <c r="G160" s="3">
+        <v>0</v>
+      </c>
+      <c r="H160" s="3">
+        <v>0</v>
+      </c>
+      <c r="I160" s="3">
+        <v>2</v>
+      </c>
+      <c r="J160" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="K160" s="3">
+        <v>0</v>
+      </c>
+      <c r="L160" s="3">
+        <v>0</v>
+      </c>
+      <c r="M160" s="3">
+        <v>25</v>
+      </c>
+      <c r="N160" s="3">
+        <v>2</v>
+      </c>
+      <c r="O160" s="3">
+        <v>33</v>
+      </c>
+      <c r="P160" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q160" s="3">
+        <v>90</v>
+      </c>
+      <c r="R160" s="3">
+        <v>60</v>
+      </c>
+      <c r="S160" s="3">
+        <v>19</v>
+      </c>
+      <c r="T160" s="3">
+        <v>8</v>
+      </c>
+      <c r="U160" s="3">
+        <v>0</v>
+      </c>
+      <c r="V160" s="3">
+        <v>44</v>
+      </c>
+      <c r="W160" s="3">
+        <v>0</v>
+      </c>
+      <c r="X160" s="3">
+        <v>5</v>
+      </c>
+      <c r="Y160" s="3">
+        <v>5</v>
+      </c>
+      <c r="Z160" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA160" s="3">
+        <v>7</v>
+      </c>
+      <c r="AB160" s="3">
+        <v>6</v>
+      </c>
+      <c r="AC160" s="3">
+        <v>5</v>
+      </c>
+      <c r="AD160" s="3">
+        <v>22</v>
+      </c>
+      <c r="AE160" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF160" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG160" s="3">
+        <v>8</v>
+      </c>
+      <c r="AH160" s="3">
+        <v>2202</v>
+      </c>
+      <c r="AI160" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ160" s="3">
+        <v>3</v>
+      </c>
+      <c r="AK160" s="3">
+        <v>66</v>
+      </c>
+      <c r="AL160" s="3">
+        <v>95</v>
+      </c>
+      <c r="AM160" s="3">
+        <v>314</v>
+      </c>
+      <c r="AN160" s="3">
+        <v>18</v>
+      </c>
+      <c r="AO160" s="3">
+        <v>12</v>
+      </c>
+      <c r="AP160" s="3">
+        <v>13</v>
+      </c>
+      <c r="AQ160" s="3">
+        <v>154</v>
+      </c>
+      <c r="AR160" s="3">
+        <v>124</v>
+      </c>
+      <c r="AS160" s="3">
+        <v>149</v>
+      </c>
+      <c r="AT160" s="3">
+        <v>137</v>
+      </c>
+      <c r="AU160" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV160" s="3">
+        <v>3</v>
+      </c>
+      <c r="AW160" s="3">
+        <v>101</v>
+      </c>
+      <c r="AX160" s="3">
+        <v>34</v>
+      </c>
+      <c r="AY160" s="3">
+        <v>43</v>
+      </c>
+      <c r="AZ160" s="3">
+        <v>103</v>
+      </c>
+      <c r="BA160" s="3">
+        <v>145</v>
+      </c>
+      <c r="BB160" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC160" s="3">
+        <v>98</v>
+      </c>
+      <c r="BD160" s="3">
+        <v>66</v>
+      </c>
+      <c r="BE160" s="3">
+        <v>0</v>
+      </c>
+      <c r="BF160" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG160" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH160" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI160" s="3">
+        <v>327</v>
+      </c>
+      <c r="BJ160" s="3">
+        <v>6</v>
+      </c>
+      <c r="BK160" s="3">
+        <v>17</v>
+      </c>
+      <c r="BL160" s="3">
+        <v>2</v>
+      </c>
+      <c r="BM160" s="3">
+        <v>173</v>
+      </c>
+      <c r="BN160" s="3">
+        <v>1636</v>
+      </c>
+      <c r="BO160" s="3">
+        <v>0</v>
+      </c>
+      <c r="BP160" s="3">
+        <v>10</v>
+      </c>
+      <c r="BQ160" s="3">
+        <v>63</v>
+      </c>
+      <c r="BR160" s="3">
+        <v>43</v>
+      </c>
+      <c r="BS160" s="3">
+        <v>384</v>
+      </c>
+      <c r="BT160" s="3">
+        <v>149</v>
+      </c>
+      <c r="BU160" s="3">
+        <v>41</v>
+      </c>
+      <c r="BV160" s="3">
+        <v>101</v>
+      </c>
+      <c r="BW160" s="3">
+        <v>0</v>
+      </c>
+      <c r="BX160" s="3">
+        <v>12</v>
+      </c>
+      <c r="BY160" s="3">
+        <v>39</v>
+      </c>
+      <c r="BZ160" s="3">
+        <v>49</v>
+      </c>
+      <c r="CA160" s="3">
+        <v>3</v>
+      </c>
+      <c r="CB160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CC160" s="3">
+        <v>55</v>
+      </c>
+      <c r="CD160" s="3">
+        <v>43</v>
+      </c>
+      <c r="CE160" s="3">
+        <v>37</v>
+      </c>
+      <c r="CF160" s="3">
+        <v>14</v>
+      </c>
+      <c r="CG160" s="3">
+        <v>16</v>
+      </c>
+      <c r="CH160" s="3">
+        <v>67</v>
+      </c>
+      <c r="CI160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CJ160" s="3">
+        <v>2</v>
+      </c>
+      <c r="CK160" s="3">
+        <v>35</v>
+      </c>
+      <c r="CL160" s="3">
+        <v>5</v>
+      </c>
+      <c r="CM160" s="3">
+        <v>206</v>
+      </c>
+      <c r="CN160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CO160" s="3">
+        <v>31</v>
+      </c>
+      <c r="CP160" s="3">
+        <v>46</v>
+      </c>
+      <c r="CQ160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CR160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CS160" s="3">
+        <v>186</v>
+      </c>
+      <c r="CT160" s="3">
+        <v>119</v>
+      </c>
+      <c r="CU160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CV160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CW160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CX160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CY160" s="3">
+        <v>0</v>
+      </c>
+      <c r="CZ160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DA160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DB160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DC160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DD160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DE160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DF160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DG160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DH160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DI160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DJ160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DK160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DL160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DM160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DN160" s="3">
+        <v>119</v>
+      </c>
+      <c r="DO160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DP160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DQ160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DR160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DS160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DT160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DU160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DV160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DW160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DX160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DY160" s="3">
+        <v>0</v>
+      </c>
+      <c r="DZ160" s="3">
+        <v>5</v>
+      </c>
+      <c r="EA160" s="3">
+        <v>26</v>
+      </c>
+      <c r="EB160" s="3">
+        <v>229</v>
+      </c>
+      <c r="EC160" s="3">
+        <v>162</v>
+      </c>
+      <c r="ED160" s="3">
+        <v>190</v>
+      </c>
+      <c r="EE160" s="3">
+        <v>116</v>
+      </c>
+      <c r="EF160" s="3">
+        <v>17</v>
+      </c>
+      <c r="EG160" s="3">
+        <v>16</v>
+      </c>
+      <c r="EH160" s="3">
+        <v>37</v>
+      </c>
+      <c r="EI160" s="3">
+        <v>462</v>
+      </c>
+      <c r="EJ160" s="3">
+        <v>251</v>
+      </c>
+      <c r="EK160" s="3">
+        <v>414</v>
+      </c>
+      <c r="EL160" s="3">
+        <v>180</v>
+      </c>
+      <c r="EM160" s="3">
+        <v>280</v>
+      </c>
+      <c r="EN160" s="3">
+        <v>525</v>
+      </c>
+      <c r="EO160" s="3">
+        <v>634</v>
+      </c>
+      <c r="EP160" s="3">
+        <v>453</v>
+      </c>
+      <c r="EQ160" s="3">
+        <v>132</v>
+      </c>
+      <c r="ER160" s="3">
+        <v>284</v>
+      </c>
+      <c r="ES160" s="3">
+        <v>127</v>
+      </c>
+      <c r="ET160" s="3">
+        <v>71</v>
+      </c>
+      <c r="EU160" s="3">
+        <v>19</v>
+      </c>
+      <c r="EV160" s="3">
+        <v>79</v>
+      </c>
+      <c r="EW160" s="3">
+        <v>24</v>
+      </c>
+      <c r="EX160" s="3">
+        <v>201</v>
+      </c>
+      <c r="EY160" s="3">
+        <v>64</v>
+      </c>
+      <c r="EZ160" s="3">
+        <v>280</v>
+      </c>
+      <c r="FA160" s="3">
+        <v>222</v>
+      </c>
+      <c r="FB160" s="3">
+        <v>98</v>
+      </c>
+      <c r="FC160" s="3">
+        <v>277</v>
+      </c>
+      <c r="FD160" s="3">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>